<commit_message>
Add subnav to layout
add content to aboutus.html, add .subnav to layout, this allows for
navigation to subpages and CTA placement
</commit_message>
<xml_diff>
--- a/website inventory.xlsx
+++ b/website inventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="17205" windowHeight="11625"/>
+    <workbookView xWindow="6975" yWindow="0" windowWidth="17205" windowHeight="11625"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="98">
   <si>
     <t>ID</t>
   </si>
@@ -983,7 +983,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,7 +1040,9 @@
       <c r="D3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="41"/>
+      <c r="E3" s="30" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">

</xml_diff>

<commit_message>
Add Play Guidelines content
Add content for play.html, clean up layout
</commit_message>
<xml_diff>
--- a/website inventory.xlsx
+++ b/website inventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6975" yWindow="0" windowWidth="17205" windowHeight="11625"/>
+    <workbookView xWindow="8370" yWindow="0" windowWidth="17205" windowHeight="11625"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
   <si>
     <t>ID</t>
   </si>
@@ -983,7 +983,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,7 +1072,9 @@
       <c r="D5" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="41"/>
+      <c r="E5" s="31" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">

</xml_diff>

<commit_message>
Add Contactus details and map
add contactus.html, add contact info and google map.
</commit_message>
<xml_diff>
--- a/website inventory.xlsx
+++ b/website inventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9765" yWindow="0" windowWidth="17205" windowHeight="11625"/>
+    <workbookView xWindow="11160" yWindow="0" windowWidth="17205" windowHeight="11625"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="98">
   <si>
     <t>ID</t>
   </si>
@@ -93,9 +93,6 @@
     <t>/index/</t>
   </si>
   <si>
-    <t>hero, cta</t>
-  </si>
-  <si>
     <t>List items</t>
   </si>
   <si>
@@ -258,12 +255,6 @@
     <t>Privacy Policy</t>
   </si>
   <si>
-    <t>/contact_us/signup/</t>
-  </si>
-  <si>
-    <t>/contact_us/privacy/</t>
-  </si>
-  <si>
     <t>Excel table intergration</t>
   </si>
   <si>
@@ -306,9 +297,6 @@
     <t>/news/</t>
   </si>
   <si>
-    <t>/news/ladder/</t>
-  </si>
-  <si>
     <t>/about_us/play/</t>
   </si>
   <si>
@@ -319,6 +307,18 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>/ladder/</t>
+  </si>
+  <si>
+    <t>/signup/</t>
+  </si>
+  <si>
+    <t>/signup/privacy/</t>
+  </si>
+  <si>
+    <t>Gallery, cta</t>
   </si>
 </sst>
 </file>
@@ -356,7 +356,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,8 +405,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -453,19 +459,6 @@
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -533,17 +526,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF000000"/>
       </left>
       <right/>
@@ -555,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -585,34 +567,25 @@
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -630,42 +603,30 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -983,7 +944,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,245 +966,251 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="24" t="s">
+      <c r="B2" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="32"/>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="40"/>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="30" t="s">
+      <c r="E8" s="33"/>
+    </row>
+    <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="30" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="41"/>
-    </row>
-    <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="41"/>
-    </row>
-    <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="41"/>
-    </row>
-    <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="41"/>
+      <c r="E9" s="33"/>
     </row>
     <row r="10" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>97</v>
-      </c>
+      <c r="E10" s="33"/>
     </row>
     <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="33"/>
+    </row>
+    <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="B12" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="35" t="s">
+    </row>
+    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="33"/>
+    </row>
+    <row r="15" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="33"/>
+    </row>
+    <row r="16" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="41"/>
-    </row>
-    <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="41"/>
-    </row>
-    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="C16" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="41"/>
-    </row>
-    <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="41"/>
-    </row>
-    <row r="15" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="41"/>
-    </row>
-    <row r="16" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" s="41"/>
+      <c r="E16" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1286,206 +1253,206 @@
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="H2" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="G4" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="G5" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add webfont Caputre it
install webfont 'capture it' apply to .silky-header h1.
</commit_message>
<xml_diff>
--- a/website inventory.xlsx
+++ b/website inventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18135" yWindow="0" windowWidth="17205" windowHeight="11625"/>
+    <workbookView xWindow="19530" yWindow="0" windowWidth="17205" windowHeight="11625" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="103">
   <si>
     <t>ID</t>
   </si>
@@ -319,6 +319,21 @@
   </si>
   <si>
     <t>Gallery, cta</t>
+  </si>
+  <si>
+    <t>favicon</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>All Pages</t>
+  </si>
+  <si>
+    <t>Logo</t>
   </si>
 </sst>
 </file>
@@ -537,36 +552,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
@@ -625,6 +620,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -942,7 +973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -965,263 +996,263 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="4" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="E2" s="32"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="16" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="16" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="16" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="16" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="16" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="6" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="6" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="6" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="6" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="25" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="21" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="22" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="23" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1233,242 +1264,275 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="7" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="29"/>
+    <col min="10" max="10" width="11.28515625" style="29" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="27" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="I1" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.3">
+      <c r="A2" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="32" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+    </row>
+    <row r="3" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="33" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="34" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="33"/>
+      <c r="D5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="28" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="34" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="30"/>
+      <c r="D7" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="34" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+    </row>
+    <row r="8" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="35"/>
+      <c r="D8" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="35" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="I8" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8" s="37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="11" t="s">
+      <c r="C9" s="37"/>
+      <c r="D9" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12" t="s">
+      <c r="F9" s="37"/>
+      <c r="G9" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>70</v>
+      <c r="H9" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="I9" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="J9" s="37" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Web font, add pictures
add picture to ladder.html, news.html,
</commit_message>
<xml_diff>
--- a/website inventory.xlsx
+++ b/website inventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20925" yWindow="0" windowWidth="17205" windowHeight="11625" activeTab="1"/>
+    <workbookView xWindow="22320" yWindow="0" windowWidth="17205" windowHeight="11625" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="117">
   <si>
     <t>ID</t>
   </si>
@@ -333,13 +333,49 @@
     <t>All Pages</t>
   </si>
   <si>
-    <t>Logo</t>
-  </si>
-  <si>
     <t>aboutus.html</t>
   </si>
   <si>
     <t>faq.html,gamerules.html</t>
+  </si>
+  <si>
+    <t>news.html</t>
+  </si>
+  <si>
+    <t>ladder.html</t>
+  </si>
+  <si>
+    <t>New name</t>
+  </si>
+  <si>
+    <t>whiteshirt.jpg</t>
+  </si>
+  <si>
+    <t>yellownet.jpg</t>
+  </si>
+  <si>
+    <t>blueshirts.jpg</t>
+  </si>
+  <si>
+    <t>sand_head.jpg</t>
+  </si>
+  <si>
+    <t>sbv_logo1.png</t>
+  </si>
+  <si>
+    <t>20 favicons</t>
+  </si>
+  <si>
+    <t>Logo - all pages</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>bluenet.jpg</t>
+  </si>
+  <si>
+    <t>really small image, grainy easly, difficult to use</t>
   </si>
 </sst>
 </file>
@@ -377,18 +413,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFBFBFB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -558,7 +588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -568,65 +598,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -636,13 +666,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -652,19 +679,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1272,10 +1312,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I2"/>
+      <selection activeCell="B3" sqref="B3:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1289,150 +1329,172 @@
     <col min="7" max="7" width="37.7109375" style="27" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.85546875" style="27" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" style="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="27"/>
+    <col min="10" max="10" width="23.85546875" style="27" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="32" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.3">
+      <c r="J1" s="38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="39" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="H2" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H3" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="28" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="G4" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="38"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H5" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="J5" s="37" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="36" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -1441,50 +1503,62 @@
       <c r="E6" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="36" t="s">
         <v>43</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H6" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="J6" s="37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="37" t="s">
+      <c r="G7" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-    </row>
-    <row r="8" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="H7" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="J7" s="39" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A8" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="36" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -1493,44 +1567,50 @@
       <c r="E8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="36" t="s">
         <v>43</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="I8" s="39" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I8" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="J8" s="37" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="36" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39" t="s">
+      <c r="E9" s="37"/>
+      <c r="F9" s="37" t="s">
         <v>71</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="I9" s="39" t="s">
+      <c r="I9" s="37" t="s">
         <v>101</v>
+      </c>
+      <c r="J9" s="37" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add thumbnails to gallery
add thumbnails to gallery and connect links, adjust breakpoint for
gallery items
</commit_message>
<xml_diff>
--- a/website inventory.xlsx
+++ b/website inventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22320" yWindow="0" windowWidth="17205" windowHeight="11625" activeTab="1"/>
+    <workbookView xWindow="23715" yWindow="0" windowWidth="17205" windowHeight="11625" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="117">
   <si>
     <t>ID</t>
   </si>
@@ -369,13 +369,13 @@
     <t>Logo - all pages</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>bluenet.jpg</t>
   </si>
   <si>
-    <t>really small image, grainy easly, difficult to use</t>
+    <t>index.html</t>
+  </si>
+  <si>
+    <t>beachnet.jpg</t>
   </si>
 </sst>
 </file>
@@ -588,7 +588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -676,15 +676,6 @@
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
@@ -695,14 +686,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1315,7 +1299,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J3"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1333,7 +1317,7 @@
     <col min="11" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -1361,7 +1345,7 @@
       <c r="I1" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="35" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1372,60 +1356,60 @@
       <c r="B2" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="37" t="s">
+      <c r="H2" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="J2" s="34" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="I3" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="J3" s="42" t="s">
+      <c r="H3" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="J3" s="34" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1433,27 +1417,33 @@
       <c r="A4" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="29" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="7" t="s">
         <v>53</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="38"/>
+      <c r="H4" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="J4" s="36" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
@@ -1462,7 +1452,7 @@
       <c r="B5" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="33" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1471,19 +1461,19 @@
       <c r="E5" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="I5" s="37" t="s">
+      <c r="H5" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="34" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1494,7 +1484,7 @@
       <c r="B6" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="33" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -1503,19 +1493,19 @@
       <c r="E6" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="33" t="s">
         <v>43</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="I6" s="37" t="s">
+      <c r="H6" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="J6" s="37" t="s">
+      <c r="J6" s="34" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1526,7 +1516,7 @@
       <c r="B7" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="33" t="s">
         <v>34</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -1535,20 +1525,20 @@
       <c r="E7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="33" t="s">
         <v>43</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H7" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="I7" s="37" t="s">
+      <c r="H7" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="J7" s="39" t="s">
-        <v>115</v>
+      <c r="J7" s="36" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -1558,7 +1548,7 @@
       <c r="B8" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="33" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -1567,19 +1557,19 @@
       <c r="E8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="33" t="s">
         <v>43</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="I8" s="37" t="s">
+      <c r="I8" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="J8" s="37" t="s">
+      <c r="J8" s="34" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1590,26 +1580,26 @@
       <c r="B9" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="33" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37" t="s">
+      <c r="E9" s="34"/>
+      <c r="F9" s="34" t="s">
         <v>71</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="H9" s="37" t="s">
+      <c r="H9" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="I9" s="37" t="s">
+      <c r="I9" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="J9" s="37" t="s">
+      <c r="J9" s="34" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>